<commit_message>
New bug found. Updated bm.xlsx
Signed-off-by: Shreyas Parbat <shreyasp.2016@sis.smu.edu.sg>
</commit_message>
<xml_diff>
--- a/metrics/bm.xlsx
+++ b/metrics/bm.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="90">
   <si>
     <t>Iteration</t>
   </si>
@@ -280,6 +280,21 @@
   </si>
   <si>
     <t>JM, Shreyas</t>
+  </si>
+  <si>
+    <t>4-7</t>
+  </si>
+  <si>
+    <t>For L2 and L3,  the SRs (at the top) are  not getting coloured</t>
+  </si>
+  <si>
+    <t>HeatMaps.jsp, L2.svg, L3.svg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Request Hetmap for L2 or L3</t>
   </si>
 </sst>
 </file>
@@ -668,7 +683,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -819,11 +834,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -833,6 +843,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1257,15 +1275,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="58"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="62"/>
       <c r="I1" s="2" t="s">
         <v>16</v>
       </c>
@@ -4428,7 +4446,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O12" sqref="O12"/>
+      <selection pane="bottomLeft" activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4939,16 +4957,16 @@
       <c r="B11" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C11" s="60" t="s">
+      <c r="C11" s="57" t="s">
         <v>79</v>
       </c>
-      <c r="D11" s="61" t="s">
+      <c r="D11" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="E11" s="60" t="s">
+      <c r="E11" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="F11" s="59" t="s">
+      <c r="F11" s="56" t="s">
         <v>82</v>
       </c>
       <c r="G11" s="36">
@@ -4960,7 +4978,7 @@
       <c r="I11" s="37">
         <v>1</v>
       </c>
-      <c r="J11" s="59" t="s">
+      <c r="J11" s="56" t="s">
         <v>33</v>
       </c>
       <c r="K11" s="32">
@@ -4969,31 +4987,53 @@
       <c r="L11" s="32">
         <v>5</v>
       </c>
-      <c r="M11" s="59" t="s">
+      <c r="M11" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="N11" s="62" t="s">
+      <c r="N11" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="O11" s="59" t="s">
+      <c r="O11" s="56" t="s">
         <v>84</v>
       </c>
       <c r="P11" s="41"/>
     </row>
     <row r="12" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="32"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="36"/>
+      <c r="A12" s="32">
+        <v>4</v>
+      </c>
+      <c r="B12" s="63" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="57" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="58" t="s">
+        <v>87</v>
+      </c>
+      <c r="E12" s="57" t="s">
+        <v>89</v>
+      </c>
+      <c r="F12" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="36">
+        <v>43024</v>
+      </c>
       <c r="H12" s="36"/>
       <c r="I12" s="37"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="32"/>
-      <c r="L12" s="32"/>
-      <c r="M12" s="38"/>
+      <c r="J12" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="K12" s="32">
+        <v>5</v>
+      </c>
+      <c r="L12" s="32">
+        <v>5</v>
+      </c>
+      <c r="M12" s="56" t="s">
+        <v>69</v>
+      </c>
       <c r="N12" s="39"/>
       <c r="O12" s="38"/>
       <c r="P12" s="41"/>
@@ -5002,7 +5042,9 @@
       <c r="A13" s="32"/>
       <c r="B13" s="33"/>
       <c r="C13" s="44"/>
-      <c r="D13" s="32"/>
+      <c r="D13" s="58" t="s">
+        <v>88</v>
+      </c>
       <c r="E13" s="44"/>
       <c r="F13" s="38"/>
       <c r="G13" s="36"/>

</xml_diff>

<commit_message>
Testing completed. Bug and task metrics updated
</commit_message>
<xml_diff>
--- a/metrics/bm.xlsx
+++ b/metrics/bm.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6072" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bug Metrics" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="279">
   <si>
     <t>Iteration</t>
   </si>
@@ -857,6 +857,18 @@
   </si>
   <si>
     <t>B1.svg, L1.svg, L2.svg, L3.svg, L4.svg, L5.svg</t>
+  </si>
+  <si>
+    <t>6-4</t>
+  </si>
+  <si>
+    <t>App Crashes when no parameters are passed for JSON student breakdown</t>
+  </si>
+  <si>
+    <t>Remove all fields when generating JSON output</t>
+  </si>
+  <si>
+    <t>MX</t>
   </si>
 </sst>
 </file>
@@ -1282,7 +1294,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1535,17 +1547,39 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1957,7 +1991,7 @@
   </sheetPr>
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -1970,15 +2004,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="G1" s="94"/>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="96"/>
       <c r="I1" s="2" t="s">
         <v>16</v>
       </c>
@@ -5139,9 +5173,9 @@
   </sheetPr>
   <dimension ref="A1:P1005"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J59" sqref="J59:J76"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M77" sqref="M77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.88671875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -6930,7 +6964,7 @@
         <v>5</v>
       </c>
       <c r="L37" s="50">
-        <f t="shared" ref="L37:L60" si="0">L36+K37</f>
+        <f t="shared" ref="L37:L58" si="0">L36+K37</f>
         <v>95</v>
       </c>
       <c r="M37" s="51" t="s">
@@ -8043,10 +8077,10 @@
       <c r="G60" s="87">
         <v>43047</v>
       </c>
-      <c r="H60" s="95">
+      <c r="H60" s="92">
         <v>43056</v>
       </c>
-      <c r="I60" s="96">
+      <c r="I60" s="93">
         <v>0.5</v>
       </c>
       <c r="J60" s="66" t="s">
@@ -8058,7 +8092,7 @@
       <c r="L60" s="83">
         <v>5</v>
       </c>
-      <c r="M60" s="96" t="s">
+      <c r="M60" s="93" t="s">
         <v>52</v>
       </c>
       <c r="N60" s="74" t="s">
@@ -8854,14 +8888,41 @@
       <c r="P76" s="41"/>
     </row>
     <row r="77" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C77" s="44"/>
-      <c r="D77" s="45"/>
-      <c r="E77" s="45"/>
-      <c r="G77" s="75"/>
-      <c r="H77" s="75"/>
-      <c r="K77" s="41"/>
-      <c r="L77" s="41"/>
-      <c r="N77" s="44"/>
+      <c r="A77" s="101">
+        <v>6</v>
+      </c>
+      <c r="B77" s="98" t="s">
+        <v>275</v>
+      </c>
+      <c r="C77" s="103" t="s">
+        <v>276</v>
+      </c>
+      <c r="D77" s="100" t="s">
+        <v>199</v>
+      </c>
+      <c r="E77" s="100" t="s">
+        <v>277</v>
+      </c>
+      <c r="F77" s="99" t="s">
+        <v>278</v>
+      </c>
+      <c r="G77" s="104">
+        <v>43058</v>
+      </c>
+      <c r="H77" s="97"/>
+      <c r="I77" s="102"/>
+      <c r="J77" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="K77" s="106">
+        <v>5</v>
+      </c>
+      <c r="L77" s="105">
+        <v>95</v>
+      </c>
+      <c r="M77" s="102"/>
+      <c r="N77" s="103"/>
+      <c r="O77" s="99"/>
       <c r="P77" s="41"/>
     </row>
     <row r="78" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Final presentation.pptx slides added. Project completed!
Signed-off-by: Shreyas Parbat <shreyasp.2016@sis.smu.edu.sg>
</commit_message>
<xml_diff>
--- a/metrics/bm.xlsx
+++ b/metrics/bm.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="287">
   <si>
     <t>Iteration</t>
   </si>
@@ -872,6 +872,27 @@
   </si>
   <si>
     <t>Edit Student breakdown json to resolve bug</t>
+  </si>
+  <si>
+    <t>6-7.1</t>
+  </si>
+  <si>
+    <t>Error Messages not sorted after token validation. If token invalid, only token error message appears but currently other fields appear too.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When all fields are invalid </t>
+  </si>
+  <si>
+    <t>Minor adjustments to json file and add collections.sort</t>
+  </si>
+  <si>
+    <t>JsonTopKCompanion.java</t>
+  </si>
+  <si>
+    <t>JsonTopNextPlaces.java</t>
+  </si>
+  <si>
+    <t>JsonTopPopularPlaces.java</t>
   </si>
 </sst>
 </file>
@@ -1297,7 +1318,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1574,11 +1595,33 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1994,7 +2037,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.88671875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2006,15 +2049,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="103" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="104"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="105"/>
       <c r="I1" s="2" t="s">
         <v>16</v>
       </c>
@@ -2139,19 +2182,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="9">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C7" s="10">
         <v>0</v>
       </c>
       <c r="D7" s="10">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="E7" s="11">
         <v>0</v>
       </c>
       <c r="F7" s="23">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="G7" s="24" t="s">
         <v>26</v>
@@ -2163,7 +2206,7 @@
       </c>
       <c r="B8" s="10">
         <f>SUM(B3:B7)</f>
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="C8" s="10">
         <f>SUM(C3:C7)</f>
@@ -2171,7 +2214,7 @@
       </c>
       <c r="D8" s="10">
         <f>SUM(D3:D7)</f>
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="E8" s="10">
         <f>SUM(E3:E7)</f>
@@ -2179,7 +2222,7 @@
       </c>
       <c r="F8" s="26">
         <f>SUM(F3:F7)</f>
-        <v>416</v>
+        <v>451</v>
       </c>
       <c r="G8" s="27"/>
     </row>
@@ -5175,9 +5218,9 @@
   </sheetPr>
   <dimension ref="A1:P1005"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E79" sqref="E79:L79"/>
+    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L84" sqref="L84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.88671875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -8914,7 +8957,7 @@
       <c r="H77" s="99">
         <v>43059</v>
       </c>
-      <c r="I77" s="105">
+      <c r="I77" s="102">
         <v>0.68</v>
       </c>
       <c r="J77" s="95" t="s">
@@ -8926,7 +8969,7 @@
       <c r="L77" s="100">
         <v>95</v>
       </c>
-      <c r="M77" s="105" t="s">
+      <c r="M77" s="102" t="s">
         <v>52</v>
       </c>
       <c r="N77" s="98" t="s">
@@ -8938,83 +8981,342 @@
       <c r="P77" s="41"/>
     </row>
     <row r="78" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C78" s="44"/>
-      <c r="D78" s="45"/>
-      <c r="E78" s="45"/>
-      <c r="G78" s="75"/>
-      <c r="H78" s="75"/>
-      <c r="K78" s="41"/>
-      <c r="L78" s="41"/>
-      <c r="N78" s="44"/>
+      <c r="A78" s="112">
+        <v>6</v>
+      </c>
+      <c r="B78" s="106" t="s">
+        <v>280</v>
+      </c>
+      <c r="C78" s="109" t="s">
+        <v>281</v>
+      </c>
+      <c r="D78" s="108" t="s">
+        <v>164</v>
+      </c>
+      <c r="E78" s="108" t="s">
+        <v>282</v>
+      </c>
+      <c r="F78" s="107" t="s">
+        <v>32</v>
+      </c>
+      <c r="G78" s="113">
+        <v>43058</v>
+      </c>
+      <c r="H78" s="113">
+        <v>43058</v>
+      </c>
+      <c r="I78" s="107">
+        <v>0.1</v>
+      </c>
+      <c r="J78" s="111" t="s">
+        <v>33</v>
+      </c>
+      <c r="K78" s="114">
+        <v>5</v>
+      </c>
+      <c r="L78" s="110">
+        <v>100</v>
+      </c>
+      <c r="M78" s="115" t="s">
+        <v>52</v>
+      </c>
+      <c r="N78" s="109" t="s">
+        <v>283</v>
+      </c>
+      <c r="O78" s="107" t="s">
+        <v>240</v>
+      </c>
       <c r="P78" s="41"/>
     </row>
     <row r="79" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C79" s="44"/>
-      <c r="D79" s="45"/>
-      <c r="E79" s="45"/>
-      <c r="G79" s="75"/>
-      <c r="H79" s="75"/>
-      <c r="K79" s="41"/>
-      <c r="L79" s="41"/>
-      <c r="N79" s="44"/>
+      <c r="A79" s="112">
+        <v>6</v>
+      </c>
+      <c r="B79" s="106" t="s">
+        <v>280</v>
+      </c>
+      <c r="C79" s="109" t="s">
+        <v>281</v>
+      </c>
+      <c r="D79" s="108" t="s">
+        <v>199</v>
+      </c>
+      <c r="E79" s="108" t="s">
+        <v>282</v>
+      </c>
+      <c r="F79" s="107" t="s">
+        <v>32</v>
+      </c>
+      <c r="G79" s="113">
+        <v>43058</v>
+      </c>
+      <c r="H79" s="113">
+        <v>43058</v>
+      </c>
+      <c r="I79" s="107">
+        <v>0.1</v>
+      </c>
+      <c r="J79" s="111" t="s">
+        <v>33</v>
+      </c>
+      <c r="K79" s="114">
+        <v>5</v>
+      </c>
+      <c r="L79" s="110">
+        <v>105</v>
+      </c>
+      <c r="M79" s="115" t="s">
+        <v>52</v>
+      </c>
+      <c r="N79" s="109" t="s">
+        <v>283</v>
+      </c>
+      <c r="O79" s="107" t="s">
+        <v>240</v>
+      </c>
       <c r="P79" s="41"/>
     </row>
     <row r="80" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C80" s="44"/>
-      <c r="D80" s="45"/>
-      <c r="E80" s="45"/>
-      <c r="G80" s="75"/>
-      <c r="H80" s="75"/>
-      <c r="K80" s="41"/>
-      <c r="L80" s="41"/>
-      <c r="N80" s="44"/>
+      <c r="A80" s="112">
+        <v>6</v>
+      </c>
+      <c r="B80" s="106" t="s">
+        <v>280</v>
+      </c>
+      <c r="C80" s="109" t="s">
+        <v>281</v>
+      </c>
+      <c r="D80" s="108" t="s">
+        <v>284</v>
+      </c>
+      <c r="E80" s="108" t="s">
+        <v>282</v>
+      </c>
+      <c r="F80" s="107" t="s">
+        <v>32</v>
+      </c>
+      <c r="G80" s="113">
+        <v>43058</v>
+      </c>
+      <c r="H80" s="113">
+        <v>43058</v>
+      </c>
+      <c r="I80" s="107">
+        <v>0.1</v>
+      </c>
+      <c r="J80" s="111" t="s">
+        <v>33</v>
+      </c>
+      <c r="K80" s="114">
+        <v>5</v>
+      </c>
+      <c r="L80" s="110">
+        <v>110</v>
+      </c>
+      <c r="M80" s="115" t="s">
+        <v>52</v>
+      </c>
+      <c r="N80" s="109" t="s">
+        <v>283</v>
+      </c>
+      <c r="O80" s="107" t="s">
+        <v>240</v>
+      </c>
       <c r="P80" s="41"/>
     </row>
-    <row r="81" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C81" s="44"/>
-      <c r="D81" s="45"/>
-      <c r="E81" s="45"/>
-      <c r="G81" s="75"/>
-      <c r="H81" s="75"/>
-      <c r="K81" s="41"/>
-      <c r="L81" s="41"/>
-      <c r="N81" s="44"/>
+    <row r="81" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="112">
+        <v>6</v>
+      </c>
+      <c r="B81" s="106" t="s">
+        <v>280</v>
+      </c>
+      <c r="C81" s="109" t="s">
+        <v>281</v>
+      </c>
+      <c r="D81" s="108" t="s">
+        <v>285</v>
+      </c>
+      <c r="E81" s="108" t="s">
+        <v>282</v>
+      </c>
+      <c r="F81" s="107" t="s">
+        <v>32</v>
+      </c>
+      <c r="G81" s="113">
+        <v>43058</v>
+      </c>
+      <c r="H81" s="113">
+        <v>43058</v>
+      </c>
+      <c r="I81" s="107">
+        <v>0.1</v>
+      </c>
+      <c r="J81" s="111" t="s">
+        <v>33</v>
+      </c>
+      <c r="K81" s="114">
+        <v>5</v>
+      </c>
+      <c r="L81" s="110">
+        <v>115</v>
+      </c>
+      <c r="M81" s="115" t="s">
+        <v>52</v>
+      </c>
+      <c r="N81" s="109" t="s">
+        <v>283</v>
+      </c>
+      <c r="O81" s="107" t="s">
+        <v>240</v>
+      </c>
       <c r="P81" s="41"/>
     </row>
-    <row r="82" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C82" s="44"/>
-      <c r="D82" s="45"/>
-      <c r="E82" s="45"/>
-      <c r="G82" s="75"/>
-      <c r="H82" s="75"/>
-      <c r="K82" s="41"/>
-      <c r="L82" s="41"/>
-      <c r="N82" s="44"/>
+    <row r="82" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="112">
+        <v>6</v>
+      </c>
+      <c r="B82" s="106" t="s">
+        <v>280</v>
+      </c>
+      <c r="C82" s="109" t="s">
+        <v>281</v>
+      </c>
+      <c r="D82" s="108" t="s">
+        <v>286</v>
+      </c>
+      <c r="E82" s="108" t="s">
+        <v>282</v>
+      </c>
+      <c r="F82" s="107" t="s">
+        <v>32</v>
+      </c>
+      <c r="G82" s="113">
+        <v>43058</v>
+      </c>
+      <c r="H82" s="113">
+        <v>43058</v>
+      </c>
+      <c r="I82" s="107">
+        <v>0.1</v>
+      </c>
+      <c r="J82" s="111" t="s">
+        <v>33</v>
+      </c>
+      <c r="K82" s="114">
+        <v>5</v>
+      </c>
+      <c r="L82" s="110">
+        <v>120</v>
+      </c>
+      <c r="M82" s="115" t="s">
+        <v>52</v>
+      </c>
+      <c r="N82" s="109" t="s">
+        <v>283</v>
+      </c>
+      <c r="O82" s="107" t="s">
+        <v>240</v>
+      </c>
       <c r="P82" s="41"/>
     </row>
-    <row r="83" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C83" s="44"/>
-      <c r="D83" s="45"/>
-      <c r="E83" s="45"/>
-      <c r="G83" s="75"/>
-      <c r="H83" s="75"/>
-      <c r="K83" s="41"/>
-      <c r="L83" s="41"/>
-      <c r="N83" s="44"/>
+    <row r="83" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="112">
+        <v>6</v>
+      </c>
+      <c r="B83" s="106" t="s">
+        <v>280</v>
+      </c>
+      <c r="C83" s="109" t="s">
+        <v>281</v>
+      </c>
+      <c r="D83" s="108" t="s">
+        <v>247</v>
+      </c>
+      <c r="E83" s="108" t="s">
+        <v>282</v>
+      </c>
+      <c r="F83" s="107" t="s">
+        <v>32</v>
+      </c>
+      <c r="G83" s="113">
+        <v>43058</v>
+      </c>
+      <c r="H83" s="113">
+        <v>43058</v>
+      </c>
+      <c r="I83" s="107">
+        <v>0.1</v>
+      </c>
+      <c r="J83" s="111" t="s">
+        <v>33</v>
+      </c>
+      <c r="K83" s="114">
+        <v>5</v>
+      </c>
+      <c r="L83" s="110">
+        <v>125</v>
+      </c>
+      <c r="M83" s="115" t="s">
+        <v>52</v>
+      </c>
+      <c r="N83" s="109" t="s">
+        <v>283</v>
+      </c>
+      <c r="O83" s="107" t="s">
+        <v>240</v>
+      </c>
       <c r="P83" s="41"/>
     </row>
-    <row r="84" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C84" s="44"/>
-      <c r="D84" s="45"/>
-      <c r="E84" s="45"/>
-      <c r="G84" s="75"/>
-      <c r="H84" s="75"/>
-      <c r="K84" s="41"/>
-      <c r="L84" s="41"/>
-      <c r="N84" s="44"/>
+    <row r="84" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="112">
+        <v>6</v>
+      </c>
+      <c r="B84" s="106" t="s">
+        <v>280</v>
+      </c>
+      <c r="C84" s="109" t="s">
+        <v>281</v>
+      </c>
+      <c r="D84" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="E84" s="108" t="s">
+        <v>282</v>
+      </c>
+      <c r="F84" s="107" t="s">
+        <v>32</v>
+      </c>
+      <c r="G84" s="113">
+        <v>43058</v>
+      </c>
+      <c r="H84" s="113">
+        <v>43058</v>
+      </c>
+      <c r="I84" s="107">
+        <v>0.1</v>
+      </c>
+      <c r="J84" s="111" t="s">
+        <v>33</v>
+      </c>
+      <c r="K84" s="114">
+        <v>5</v>
+      </c>
+      <c r="L84" s="110">
+        <v>130</v>
+      </c>
+      <c r="M84" s="115" t="s">
+        <v>52</v>
+      </c>
+      <c r="N84" s="109" t="s">
+        <v>283</v>
+      </c>
+      <c r="O84" s="107" t="s">
+        <v>240</v>
+      </c>
       <c r="P84" s="41"/>
     </row>
-    <row r="85" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C85" s="44"/>
       <c r="D85" s="45"/>
       <c r="E85" s="45"/>
@@ -9025,7 +9327,7 @@
       <c r="N85" s="44"/>
       <c r="P85" s="41"/>
     </row>
-    <row r="86" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C86" s="44"/>
       <c r="D86" s="45"/>
       <c r="E86" s="45"/>
@@ -9036,7 +9338,7 @@
       <c r="N86" s="44"/>
       <c r="P86" s="41"/>
     </row>
-    <row r="87" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C87" s="44"/>
       <c r="D87" s="45"/>
       <c r="E87" s="45"/>
@@ -9047,7 +9349,7 @@
       <c r="N87" s="44"/>
       <c r="P87" s="41"/>
     </row>
-    <row r="88" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C88" s="44"/>
       <c r="D88" s="45"/>
       <c r="E88" s="45"/>
@@ -9058,7 +9360,7 @@
       <c r="N88" s="44"/>
       <c r="P88" s="41"/>
     </row>
-    <row r="89" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C89" s="44"/>
       <c r="D89" s="45"/>
       <c r="E89" s="45"/>
@@ -9069,7 +9371,7 @@
       <c r="N89" s="44"/>
       <c r="P89" s="41"/>
     </row>
-    <row r="90" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C90" s="44"/>
       <c r="D90" s="45"/>
       <c r="E90" s="45"/>
@@ -9080,7 +9382,7 @@
       <c r="N90" s="44"/>
       <c r="P90" s="41"/>
     </row>
-    <row r="91" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C91" s="44"/>
       <c r="D91" s="45"/>
       <c r="E91" s="45"/>
@@ -9091,7 +9393,7 @@
       <c r="N91" s="44"/>
       <c r="P91" s="41"/>
     </row>
-    <row r="92" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C92" s="44"/>
       <c r="D92" s="45"/>
       <c r="E92" s="45"/>
@@ -9102,7 +9404,7 @@
       <c r="N92" s="44"/>
       <c r="P92" s="41"/>
     </row>
-    <row r="93" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C93" s="44"/>
       <c r="D93" s="45"/>
       <c r="E93" s="45"/>
@@ -9113,7 +9415,7 @@
       <c r="N93" s="44"/>
       <c r="P93" s="41"/>
     </row>
-    <row r="94" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C94" s="44"/>
       <c r="D94" s="45"/>
       <c r="E94" s="45"/>
@@ -9124,7 +9426,7 @@
       <c r="N94" s="44"/>
       <c r="P94" s="41"/>
     </row>
-    <row r="95" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C95" s="44"/>
       <c r="D95" s="45"/>
       <c r="E95" s="45"/>
@@ -9135,7 +9437,7 @@
       <c r="N95" s="44"/>
       <c r="P95" s="41"/>
     </row>
-    <row r="96" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C96" s="44"/>
       <c r="D96" s="45"/>
       <c r="E96" s="45"/>

</xml_diff>